<commit_message>
Added some MDOP packages to list
</commit_message>
<xml_diff>
--- a/Windows 10 Features.xlsx
+++ b/Windows 10 Features.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvin\Documents\GitHub\SOE Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvin\Documents\GitHub\Windows10-Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="50">
   <si>
     <t>Windows 10 Features</t>
   </si>
@@ -152,6 +152,30 @@
   </si>
   <si>
     <t>Adobe Flash Player v13.0.0.0</t>
+  </si>
+  <si>
+    <t>User Experience Virtualization</t>
+  </si>
+  <si>
+    <t>MBAM</t>
+  </si>
+  <si>
+    <t>DaRT</t>
+  </si>
+  <si>
+    <t>MDOP: UE-V</t>
+  </si>
+  <si>
+    <t>Installed</t>
+  </si>
+  <si>
+    <t>Not Installed</t>
+  </si>
+  <si>
+    <t>MDOP: MBAM</t>
+  </si>
+  <si>
+    <t>MDOP: DaRT</t>
   </si>
 </sst>
 </file>
@@ -602,7 +626,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D16"/>
+  <dimension ref="B2:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -745,16 +769,71 @@
         <v>37</v>
       </c>
     </row>
+    <row r="18" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B18" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+    </row>
+    <row r="19" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" t="str">
+        <f>VLOOKUP(C20,Data!B30:C31,2,FALSE)</f>
+        <v>Notes</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" t="str">
+        <f>VLOOKUP(C21,Data!B34:C35,2,FALSE)</f>
+        <v>Notes</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" t="str">
+        <f>VLOOKUP(C22,Data!B38:C39,2,FALSE)</f>
+        <v>Notes</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Data!$B$3:$B$6</xm:f>
@@ -791,6 +870,24 @@
           </x14:formula1>
           <xm:sqref>C15</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Data!$B$30:$B$31</xm:f>
+          </x14:formula1>
+          <xm:sqref>C20</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Data!$B$34:$B$35</xm:f>
+          </x14:formula1>
+          <xm:sqref>C21</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Data!$B$38:$B$39</xm:f>
+          </x14:formula1>
+          <xm:sqref>C22</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -799,10 +896,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C27"/>
+  <dimension ref="B2:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,7 +1038,7 @@
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>38</v>
       </c>
     </row>
@@ -959,6 +1056,69 @@
       </c>
       <c r="C27" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>